<commit_message>
Added sowing per treatment
</commit_message>
<xml_diff>
--- a/WindowsClient/Data/Demo_2_Experiments.xlsx
+++ b/WindowsClient/Data/Demo_2_Experiments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Apsim\REMS\REMS2020\WindowsClient\bin\Debug\netcoreapp3.0\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Apsim\REMS\REMS2020\WindowsClient\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43841411-A397-4798-9A90-1A7C52AD1DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421F3256-CDF4-4A0A-AC03-196CF9910AA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37410" yWindow="1380" windowWidth="28215" windowHeight="14205" tabRatio="669" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18765" yWindow="2850" windowWidth="21285" windowHeight="13725" tabRatio="669" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="20" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="69">
   <si>
     <t>Notes</t>
   </si>
@@ -232,18 +232,18 @@
   <si>
     <t>20</t>
   </si>
+  <si>
+    <t>ATX623xRTX430</t>
+  </si>
+  <si>
+    <t>QL41xQL36</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -276,6 +276,10 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -5582,10 +5586,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B147167-1129-4539-A51B-327E0C86BF99}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5605,7 +5609,7 @@
         <v>53</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>1</v>
@@ -5631,7 +5635,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23">
-        <v>202</v>
+        <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>56</v>
@@ -5657,13 +5661,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="23">
-        <v>203</v>
+        <v>2</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>57</v>
@@ -5678,7 +5682,580 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="23">
+        <v>4</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="23">
+        <v>5</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="23">
+        <v>7</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23">
+        <v>8</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="23">
+        <v>10</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="23">
+        <v>11</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14" s="23">
+        <v>13</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23">
+        <v>14</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="23">
+        <v>16</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18" s="23">
+        <v>17</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="23">
+        <v>19</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="23">
+        <v>20</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="23">
+        <v>23</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="27">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
adding names to treatments
</commit_message>
<xml_diff>
--- a/WindowsClient/Data/Demo_2_Experiments.xlsx
+++ b/WindowsClient/Data/Demo_2_Experiments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Apsim\REMS\REMS2020\WindowsClient\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\websites\trials\REMS2020\WindowsClient\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421F3256-CDF4-4A0A-AC03-196CF9910AA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED9FCD6-2FC6-4D8D-9A62-B70702123C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18765" yWindow="2850" windowWidth="21285" windowHeight="13725" tabRatio="669" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23325" yWindow="5010" windowWidth="22545" windowHeight="15135" tabRatio="669" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="20" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="81">
   <si>
     <t>Notes</t>
   </si>
@@ -237,6 +237,42 @@
   </si>
   <si>
     <t>QL41xQL36</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
   </si>
 </sst>
 </file>
@@ -2673,7 +2709,7 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3342,7 +3378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3367,6 +3405,9 @@
       <c r="B2" s="2">
         <v>202</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -3375,6 +3416,9 @@
       <c r="B3" s="2">
         <v>202</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -3383,6 +3427,9 @@
       <c r="B4" s="2">
         <v>202</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -3391,6 +3438,9 @@
       <c r="B5" s="2">
         <v>202</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -3399,6 +3449,9 @@
       <c r="B6" s="2">
         <v>202</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -3407,6 +3460,9 @@
       <c r="B7" s="2">
         <v>202</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -3415,6 +3471,9 @@
       <c r="B8" s="2">
         <v>202</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -3423,6 +3482,9 @@
       <c r="B9" s="2">
         <v>202</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -3431,6 +3493,9 @@
       <c r="B10" s="2">
         <v>202</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -3439,6 +3504,9 @@
       <c r="B11" s="2">
         <v>202</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -3447,6 +3515,9 @@
       <c r="B12" s="2">
         <v>202</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -3455,6 +3526,9 @@
       <c r="B13" s="2">
         <v>202</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -3463,6 +3537,9 @@
       <c r="B14" s="2">
         <v>203</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -3471,6 +3548,9 @@
       <c r="B15" s="2">
         <v>203</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -3479,80 +3559,111 @@
       <c r="B16" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>203</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>203</v>
       </c>
+      <c r="C25" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5588,7 +5699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B147167-1129-4539-A51B-327E0C86BF99}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>